<commit_message>
Descriptive + ANOVA + Linear Regression
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pramod\Desktop\Pramod\2020\Publications\Noha\Manure data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simba/Dharma/Ideas&amp;Projects/Academic/Projects/Dairy_Agroecosystems/Analysis/GitHub/DairyEffluents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3ACA3B-6E76-40C2-AB27-207DDD05EF5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7470806A-7B38-4C43-A52E-B098BEE8DFA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D-ions" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="TS-VS" sheetId="2" r:id="rId3"/>
     <sheet name="bacterial Jerry results" sheetId="4" r:id="rId4"/>
     <sheet name="bacterial Dennis results" sheetId="5" r:id="rId5"/>
+    <sheet name="Updated Bact Data (C samples)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="140">
   <si>
     <t>Ions</t>
   </si>
@@ -377,6 +378,78 @@
   </si>
   <si>
     <t>VS % (percentage of total solids)</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>J12</t>
   </si>
 </sst>
 </file>
@@ -468,7 +541,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -491,11 +564,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -561,6 +660,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,14 +954,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="12"/>
-    <col min="2" max="2" width="8.7109375" style="5"/>
-    <col min="3" max="16384" width="8.7109375" style="3"/>
+    <col min="1" max="1" width="8.6640625" style="12"/>
+    <col min="2" max="2" width="8.6640625" style="5"/>
+    <col min="3" max="16384" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1110,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>0.08</v>
       </c>
@@ -1149,7 +1256,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
@@ -1298,7 +1405,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>0.08</v>
       </c>
@@ -1444,7 +1551,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>180</v>
       </c>
@@ -1590,7 +1697,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>2</v>
       </c>
@@ -1739,7 +1846,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>230</v>
       </c>
@@ -1885,7 +1992,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>380</v>
       </c>
@@ -2031,7 +2138,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="14" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
@@ -2180,7 +2287,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>380</v>
       </c>
@@ -2326,7 +2433,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="18" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>540</v>
       </c>
@@ -2472,7 +2579,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>4</v>
       </c>
@@ -2621,7 +2728,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
         <v>550</v>
       </c>
@@ -2767,7 +2874,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="23" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
         <v>400</v>
       </c>
@@ -2913,7 +3020,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="24" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>5</v>
       </c>
@@ -3062,7 +3169,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>410</v>
       </c>
@@ -3208,7 +3315,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="28" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>7.3</v>
       </c>
@@ -3354,7 +3461,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="29" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>6</v>
       </c>
@@ -3503,7 +3610,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="30" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
         <v>7</v>
       </c>
@@ -3649,7 +3756,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="33" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
         <v>1.4</v>
       </c>
@@ -3792,7 +3899,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="34" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>7</v>
       </c>
@@ -3938,7 +4045,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="35" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B35" s="5">
         <v>1.2</v>
       </c>
@@ -4096,12 +4203,12 @@
       <selection sqref="A1:BH35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="19"/>
+    <col min="1" max="16384" width="8.6640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4250,11 +4357,11 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
     </row>
-    <row r="3" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="16">
         <v>0.04</v>
@@ -4401,7 +4508,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
@@ -4550,7 +4657,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
       <c r="B5" s="16">
         <v>0.04</v>
@@ -4697,15 +4804,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
     </row>
-    <row r="7" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
     </row>
-    <row r="8" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="15"/>
       <c r="B8" s="16">
         <v>230</v>
@@ -4852,7 +4959,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>2</v>
       </c>
@@ -5001,7 +5108,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
       <c r="B10" s="16">
         <v>250</v>
@@ -5148,15 +5255,15 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
     </row>
-    <row r="13" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
       <c r="B13" s="16">
         <v>650</v>
@@ -5303,7 +5410,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="14" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>3</v>
       </c>
@@ -5452,7 +5559,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="15"/>
       <c r="B15" s="16">
         <v>680</v>
@@ -5599,15 +5706,15 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
     </row>
-    <row r="17" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
       <c r="B17" s="16"/>
     </row>
-    <row r="18" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
       <c r="B18" s="16">
         <v>280</v>
@@ -5754,7 +5861,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>4</v>
       </c>
@@ -5903,7 +6010,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="20" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
       <c r="B20" s="16">
         <v>300</v>
@@ -6050,15 +6157,15 @@
         <v>420</v>
       </c>
     </row>
-    <row r="21" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
     </row>
-    <row r="22" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="16"/>
     </row>
-    <row r="23" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
       <c r="B23" s="16">
         <v>1700</v>
@@ -6205,7 +6312,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="24" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>5</v>
       </c>
@@ -6354,7 +6461,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="25" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="16">
         <v>1500</v>
@@ -6501,15 +6608,15 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="26" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
       <c r="B26" s="16"/>
     </row>
-    <row r="27" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
       <c r="B27" s="16"/>
     </row>
-    <row r="28" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
       <c r="B28" s="16">
         <v>7.1</v>
@@ -6656,7 +6763,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="29" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>6</v>
       </c>
@@ -6805,7 +6912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
       <c r="B30" s="16">
         <v>7</v>
@@ -6952,15 +7059,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
       <c r="B31" s="16"/>
     </row>
-    <row r="32" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
       <c r="B32" s="16"/>
     </row>
-    <row r="33" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
       <c r="B33" s="16">
         <v>1.3</v>
@@ -7107,7 +7214,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="34" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
         <v>7</v>
       </c>
@@ -7257,7 +7364,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="35" spans="1:60" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:60" s="17" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A35" s="15"/>
       <c r="B35" s="16">
         <v>1.4</v>
@@ -7413,19 +7520,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7180391-60B7-40A5-B41F-032E508AA5A3}">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -7436,7 +7543,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -7447,7 +7554,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -7458,7 +7565,7 @@
         <v>24.999999999999446</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -7469,7 +7576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -7480,7 +7587,7 @@
         <v>77.272727272727323</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -7491,7 +7598,7 @@
         <v>26.666666666666472</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -7502,7 +7609,7 @@
         <v>17.499999999999908</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -7513,7 +7620,7 @@
         <v>85.806451612903089</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -7524,7 +7631,7 @@
         <v>60.000000000000711</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -7535,7 +7642,7 @@
         <v>21.66666666666632</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -7546,7 +7653,7 @@
         <v>21.111111111109313</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -7557,7 +7664,7 @@
         <v>32.489451476793221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -7568,7 +7675,7 @@
         <v>15.000000000000888</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -7579,7 +7686,7 @@
         <v>14.772727272727296</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -7590,7 +7697,7 @@
         <v>24.444444444444752</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -7601,7 +7708,7 @@
         <v>90.052356020942383</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -7612,7 +7719,7 @@
         <v>11.904761904762635</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -7623,7 +7730,7 @@
         <v>67.045454545454675</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
@@ -7634,7 +7741,7 @@
         <v>62.26415094339427</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
@@ -7645,7 +7752,7 @@
         <v>53.30396475770938</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -7656,7 +7763,7 @@
         <v>54.545454545456018</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
@@ -7667,7 +7774,7 @@
         <v>62.162162162161451</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
@@ -7678,7 +7785,7 @@
         <v>38.461538461540037</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -7689,7 +7796,7 @@
         <v>88.343558282208534</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -7700,7 +7807,7 @@
         <v>29.629629629627193</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>37</v>
       </c>
@@ -7711,7 +7818,7 @@
         <v>40.909090909092008</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
@@ -7722,7 +7829,7 @@
         <v>39.393939393939718</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>39</v>
       </c>
@@ -7733,7 +7840,7 @@
         <v>88.025889967637312</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>40</v>
       </c>
@@ -7744,7 +7851,7 @@
         <v>46.33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>41</v>
       </c>
@@ -7756,7 +7863,7 @@
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>42</v>
       </c>
@@ -7767,7 +7874,7 @@
         <v>11.666666666666197</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>43</v>
       </c>
@@ -7778,7 +7885,7 @@
         <v>57.751277683134596</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>44</v>
       </c>
@@ -7790,7 +7897,7 @@
       </c>
       <c r="F33" s="23"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>45</v>
       </c>
@@ -7802,7 +7909,7 @@
       </c>
       <c r="F34" s="23"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>46</v>
       </c>
@@ -7815,7 +7922,7 @@
       <c r="F35" s="23"/>
       <c r="H35" s="23"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>47</v>
       </c>
@@ -7827,7 +7934,7 @@
       </c>
       <c r="F36" s="23"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>48</v>
       </c>
@@ -7838,7 +7945,7 @@
         <v>83.333333333333584</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>49</v>
       </c>
@@ -7849,7 +7956,7 @@
         <v>25.64102564102614</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>50</v>
       </c>
@@ -7860,7 +7967,7 @@
         <v>35.714285714286511</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>51</v>
       </c>
@@ -7871,7 +7978,7 @@
         <v>45.454545454544906</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>52</v>
       </c>
@@ -7882,7 +7989,7 @@
         <v>32.894736842104727</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>53</v>
       </c>
@@ -7893,7 +8000,7 @@
         <v>76.677316293929636</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>54</v>
       </c>
@@ -7904,7 +8011,7 @@
         <v>9.9667774086379524</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>55</v>
       </c>
@@ -7915,7 +8022,7 @@
         <v>11.904761904762076</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>56</v>
       </c>
@@ -7926,7 +8033,7 @@
         <v>51.546391752576916</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
@@ -7937,7 +8044,7 @@
         <v>61.53846153846122</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>58</v>
       </c>
@@ -7948,7 +8055,7 @@
         <v>39.999999999998579</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>59</v>
       </c>
@@ -7959,7 +8066,7 @@
         <v>27.653631284916287</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>60</v>
       </c>
@@ -7970,7 +8077,7 @@
         <v>60.396039603960347</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>61</v>
       </c>
@@ -7981,7 +8088,7 @@
         <v>49.999999999995559</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>62</v>
       </c>
@@ -7992,7 +8099,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>63</v>
       </c>
@@ -8003,7 +8110,7 @@
         <v>5.3627760252367001</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>64</v>
       </c>
@@ -8014,7 +8121,7 @@
         <v>43.66197183098636</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>93</v>
       </c>
@@ -8025,7 +8132,7 @@
         <v>36.708860759494101</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>94</v>
       </c>
@@ -8036,7 +8143,7 @@
         <v>32.608695652173346</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>95</v>
       </c>
@@ -8047,7 +8154,7 @@
         <v>75.471698113207708</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>96</v>
       </c>
@@ -8058,7 +8165,7 @@
         <v>44.444444444443562</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>81</v>
       </c>
@@ -8069,7 +8176,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>82</v>
       </c>
@@ -8080,7 +8187,7 @@
         <v>8.3333333333331474</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>83</v>
       </c>
@@ -8091,7 +8198,7 @@
         <v>7.874015748031324</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>84</v>
       </c>
@@ -8102,7 +8209,7 @@
         <v>47.422680412370724</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>101</v>
       </c>
@@ -8113,7 +8220,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>102</v>
       </c>
@@ -8124,7 +8231,7 @@
         <v>60.000000000000711</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>103</v>
       </c>
@@ -8135,7 +8242,7 @@
         <v>14.525139664804337</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>104</v>
       </c>
@@ -8146,7 +8253,7 @@
         <v>22.727272727272819</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>65</v>
       </c>
@@ -8157,7 +8264,7 @@
         <v>55.284552845528324</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>66</v>
       </c>
@@ -8168,7 +8275,7 @@
         <v>45.736434108527085</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>67</v>
       </c>
@@ -8179,7 +8286,7 @@
         <v>70.370370370370352</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>68</v>
       </c>
@@ -8190,7 +8297,7 @@
         <v>60.402684563758278</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>69</v>
       </c>
@@ -8201,7 +8308,7 @@
         <v>51.948051948051877</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>70</v>
       </c>
@@ -8212,7 +8319,7 @@
         <v>35.555555555555557</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>71</v>
       </c>
@@ -8223,7 +8330,7 @@
         <v>69.642857142857167</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>72</v>
       </c>
@@ -8234,7 +8341,7 @@
         <v>14.285714285714739</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>73</v>
       </c>
@@ -8245,7 +8352,7 @@
         <v>53.846153846153769</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>74</v>
       </c>
@@ -8256,7 +8363,7 @@
         <v>36.585365853658537</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>75</v>
       </c>
@@ -8267,7 +8374,7 @@
         <v>68.493150684931507</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>76</v>
       </c>
@@ -8278,7 +8385,7 @@
         <v>57.692307692307601</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>89</v>
       </c>
@@ -8289,7 +8396,7 @@
         <v>34.408602150537675</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>90</v>
       </c>
@@ -8300,7 +8407,7 @@
         <v>23.529411764705912</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>91</v>
       </c>
@@ -8311,7 +8418,7 @@
         <v>16.000000000000014</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>92</v>
       </c>
@@ -8322,7 +8429,7 @@
         <v>39.473684210526372</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>85</v>
       </c>
@@ -8333,7 +8440,7 @@
         <v>15.000000000000027</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>86</v>
       </c>
@@ -8344,7 +8451,7 @@
         <v>26.548672566371511</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>87</v>
       </c>
@@ -8355,7 +8462,7 @@
         <v>22.259259259259274</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>88</v>
       </c>
@@ -8366,7 +8473,7 @@
         <v>21.088435374149601</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>77</v>
       </c>
@@ -8377,7 +8484,7 @@
         <v>12.658227848101273</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>78</v>
       </c>
@@ -8388,7 +8495,7 @@
         <v>16.666666666666682</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>79</v>
       </c>
@@ -8399,7 +8506,7 @@
         <v>15.121951219512159</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>80</v>
       </c>
@@ -8424,14 +8531,14 @@
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="8.7109375" style="19"/>
-    <col min="4" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="19"/>
+    <col min="1" max="3" width="8.6640625" style="19"/>
+    <col min="4" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>105</v>
       </c>
@@ -8454,7 +8561,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
@@ -8474,7 +8581,7 @@
         <v>916.51513899116799</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>58</v>
       </c>
@@ -8494,7 +8601,7 @@
         <v>1331.6656236958784</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>60</v>
       </c>
@@ -8514,7 +8621,7 @@
         <v>456.2163229580168</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>61</v>
       </c>
@@ -8539,7 +8646,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>62</v>
       </c>
@@ -8564,7 +8671,7 @@
         <v>847.91410728524465</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>64</v>
       </c>
@@ -8589,7 +8696,7 @@
         <v>847.63887751014977</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>65</v>
       </c>
@@ -8614,7 +8721,7 @@
         <v>13222.465730717549</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
@@ -8639,7 +8746,7 @@
         <v>694.47222166668894</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>68</v>
       </c>
@@ -8661,7 +8768,7 @@
         <v>6017.7515180782702</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>69</v>
       </c>
@@ -8685,7 +8792,7 @@
         <v>424.26406871192853</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>70</v>
       </c>
@@ -8709,7 +8816,7 @@
         <v>47.258156262526086</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>72</v>
       </c>
@@ -8733,7 +8840,7 @@
         <v>288.67513459481285</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>73</v>
       </c>
@@ -8758,7 +8865,7 @@
         <v>6443.7482622047446</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>74</v>
       </c>
@@ -8783,7 +8890,7 @@
         <v>3836.2612007004946</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>76</v>
       </c>
@@ -8808,7 +8915,7 @@
         <v>4830.276044561705</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>77</v>
       </c>
@@ -8833,7 +8940,7 @@
         <v>1757.6783930325062</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>78</v>
       </c>
@@ -8858,7 +8965,7 @@
         <v>3711.3193970159273</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>80</v>
       </c>
@@ -8883,7 +8990,7 @@
         <v>2267.6621588470066</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>81</v>
       </c>
@@ -8908,7 +9015,7 @@
         <v>8551.6080359193256</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>82</v>
       </c>
@@ -8933,7 +9040,7 @@
         <v>529.02425905308598</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>84</v>
       </c>
@@ -8958,7 +9065,7 @@
         <v>680.68592855540453</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>85</v>
       </c>
@@ -8983,7 +9090,7 @@
         <v>6553.0857871184116</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -9008,7 +9115,7 @@
         <v>558.33084576560282</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>88</v>
       </c>
@@ -9033,7 +9140,7 @@
         <v>495.04208575298588</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>89</v>
       </c>
@@ -9058,7 +9165,7 @@
         <v>253.37718918639854</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>90</v>
       </c>
@@ -9083,7 +9190,7 @@
         <v>784.07057505473745</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>92</v>
       </c>
@@ -9108,7 +9215,7 @@
         <v>378.18646194701364</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>93</v>
       </c>
@@ -9133,7 +9240,7 @@
         <v>1546.6954020319147</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>94</v>
       </c>
@@ -9158,7 +9265,7 @@
         <v>1348.0696075005426</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>96</v>
       </c>
@@ -9183,7 +9290,7 @@
         <v>3716.3187430574358</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>97</v>
       </c>
@@ -9208,7 +9315,7 @@
         <v>1555.1071774425495</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>98</v>
       </c>
@@ -9233,7 +9340,7 @@
         <v>904.13863243789478</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>100</v>
       </c>
@@ -9253,7 +9360,7 @@
         <v>3978.0062007660736</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>101</v>
       </c>
@@ -9278,7 +9385,7 @@
         <v>3155.7988951558154</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>102</v>
       </c>
@@ -9303,7 +9410,7 @@
         <v>6475.9162800847471</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>104</v>
       </c>
@@ -9341,9 +9448,9 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>105</v>
       </c>
@@ -9366,7 +9473,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>106</v>
       </c>
@@ -9389,7 +9496,7 @@
         <v>51.881274720911264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>107</v>
       </c>
@@ -9412,7 +9519,7 @@
         <v>46.188021535170066</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>108</v>
       </c>
@@ -9435,7 +9542,7 @@
         <v>64.031242374328485</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -9458,7 +9565,7 @@
         <v>41.129875597510221</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -9481,7 +9588,7 @@
         <v>60.759087111860616</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -9504,7 +9611,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -9527,7 +9634,7 @@
         <v>32.015621187164243</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -9550,7 +9657,7 @@
         <v>1201.8319350058891</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -9573,7 +9680,7 @@
         <v>48.989794855663561</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -9596,7 +9703,7 @@
         <v>1448.7695929074898</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -9619,7 +9726,7 @@
         <v>1449.1376746189439</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -9642,7 +9749,7 @@
         <v>102.42883708539635</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -9665,7 +9772,7 @@
         <v>1350.145053935564</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -9688,7 +9795,7 @@
         <v>865.544144839919</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -9711,7 +9818,7 @@
         <v>7.0710678118654755</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -9734,7 +9841,7 @@
         <v>602.07972893961482</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
@@ -9757,7 +9864,7 @@
         <v>675.15430335096983</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -9780,7 +9887,7 @@
         <v>86.602540378443862</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -9803,7 +9910,7 @@
         <v>823.97410962562003</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
@@ -9826,7 +9933,7 @@
         <v>1915.3676757566243</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
@@ -9849,7 +9956,7 @@
         <v>692.8203230275509</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>37</v>
       </c>
@@ -9872,7 +9979,7 @@
         <v>967.38479072876339</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>38</v>
       </c>
@@ -9895,7 +10002,7 @@
         <v>2299.6231575340048</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
@@ -9918,7 +10025,7 @@
         <v>45.734742446707479</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>41</v>
       </c>
@@ -9941,7 +10048,7 @@
         <v>1661.5956186750132</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>42</v>
       </c>
@@ -9964,7 +10071,7 @@
         <v>927.36184954957037</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>44</v>
       </c>
@@ -9987,7 +10094,7 @@
         <v>196.19293225462192</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
@@ -10010,7 +10117,7 @@
         <v>1397.2830779766855</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>46</v>
       </c>
@@ -10033,7 +10140,7 @@
         <v>707.54858490424533</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>48</v>
       </c>
@@ -10056,7 +10163,7 @@
         <v>577.35026918962569</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
@@ -10079,7 +10186,7 @@
         <v>962.68721123045293</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>50</v>
       </c>
@@ -10102,7 +10209,7 @@
         <v>421.06016988865935</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>52</v>
       </c>
@@ -10125,7 +10232,7 @@
         <v>676.92934146285404</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>53</v>
       </c>
@@ -10148,7 +10255,7 @@
         <v>496.78969393496885</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>54</v>
       </c>
@@ -10171,7 +10278,7 @@
         <v>1215.1817422372123</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>56</v>
       </c>
@@ -10192,6 +10299,277 @@
       </c>
       <c r="H37">
         <v>996.60674290313727</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7208C90-BCC0-FD4C-97C1-AAFADBEA3800}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3">
+        <v>88</v>
+      </c>
+      <c r="E2" s="3">
+        <v>176</v>
+      </c>
+      <c r="F2" s="3">
+        <v>240</v>
+      </c>
+      <c r="G2" s="3">
+        <v>260</v>
+      </c>
+      <c r="H2" s="3">
+        <v>140</v>
+      </c>
+      <c r="I2" s="3">
+        <v>280</v>
+      </c>
+      <c r="J2" s="3">
+        <v>144</v>
+      </c>
+      <c r="K2" s="3">
+        <v>160</v>
+      </c>
+      <c r="L2" s="3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
+        <v>20</v>
+      </c>
+      <c r="B3" s="25">
+        <v>35</v>
+      </c>
+      <c r="C3" s="25">
+        <v>40</v>
+      </c>
+      <c r="D3" s="25">
+        <v>100</v>
+      </c>
+      <c r="E3" s="25">
+        <v>188</v>
+      </c>
+      <c r="F3" s="25">
+        <v>240</v>
+      </c>
+      <c r="G3" s="25">
+        <v>284</v>
+      </c>
+      <c r="H3" s="25">
+        <v>156</v>
+      </c>
+      <c r="I3" s="25">
+        <v>266</v>
+      </c>
+      <c r="J3" s="25">
+        <v>160</v>
+      </c>
+      <c r="K3" s="25">
+        <v>170</v>
+      </c>
+      <c r="L3" s="25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="28">
+        <v>24</v>
+      </c>
+      <c r="B7" s="28">
+        <v>3</v>
+      </c>
+      <c r="C7" s="28">
+        <v>104</v>
+      </c>
+      <c r="D7" s="28">
+        <v>36</v>
+      </c>
+      <c r="E7" s="28">
+        <v>100</v>
+      </c>
+      <c r="F7" s="28">
+        <v>140</v>
+      </c>
+      <c r="G7" s="28">
+        <v>200</v>
+      </c>
+      <c r="H7" s="28">
+        <v>144</v>
+      </c>
+      <c r="I7" s="28">
+        <v>168</v>
+      </c>
+      <c r="J7" s="28">
+        <v>240</v>
+      </c>
+      <c r="K7" s="28">
+        <v>104</v>
+      </c>
+      <c r="L7" s="28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="28">
+        <v>35</v>
+      </c>
+      <c r="B8" s="28">
+        <v>2</v>
+      </c>
+      <c r="C8" s="28">
+        <v>100</v>
+      </c>
+      <c r="D8" s="28">
+        <v>45</v>
+      </c>
+      <c r="E8" s="28">
+        <v>120</v>
+      </c>
+      <c r="F8" s="28">
+        <v>164</v>
+      </c>
+      <c r="G8" s="28">
+        <v>200</v>
+      </c>
+      <c r="H8" s="28">
+        <v>165</v>
+      </c>
+      <c r="I8" s="28">
+        <v>180</v>
+      </c>
+      <c r="J8" s="28">
+        <v>200</v>
+      </c>
+      <c r="K8" s="28">
+        <v>112</v>
+      </c>
+      <c r="L8" s="28">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>